<commit_message>
Rebuild flow map logic and data pipeline
</commit_message>
<xml_diff>
--- a/backend/data/atlas/processed/Finra/finra_congress.xlsx
+++ b/backend/data/atlas/processed/Finra/finra_congress.xlsx
@@ -1358,16 +1358,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1383,7 +1375,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1391,30 +1383,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1716,25 +1690,25 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>